<commit_message>
Added Email Address to SubmitPPIPayment request data
</commit_message>
<xml_diff>
--- a/ACHabusePolicy.xlsx
+++ b/ACHabusePolicy.xlsx
@@ -1,22 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\SoapData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16C7CD89-C0D0-40CA-A19A-913B211B06A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31C8CAE3-759F-4218-882E-649D86A82226}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30855" yWindow="510" windowWidth="19830" windowHeight="15195" activeTab="2" xr2:uid="{D8D13C30-BCF2-4971-B336-2A193264511C}"/>
+    <workbookView xWindow="1380" yWindow="2810" windowWidth="31880" windowHeight="14900" xr2:uid="{D8D13C30-BCF2-4971-B336-2A193264511C}"/>
   </bookViews>
   <sheets>
     <sheet name="SubmitPayment" sheetId="1" r:id="rId1"/>
     <sheet name="SubmitPaymentWallet" sheetId="2" r:id="rId2"/>
     <sheet name="SubmitPaymentNegative" sheetId="3" r:id="rId3"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">SubmitPayment!$H$1:$H$28</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -266,7 +269,7 @@
   </cellStyleXfs>
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -591,24 +594,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5EBB363B-B62F-42A3-A89D-99F2C4FC4A0B}">
   <dimension ref="A1:H28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.15234375" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="1" max="1" width="10" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.3828125" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.3046875" style="2" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="15" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="9" max="16384" width="9.140625" style="2"/>
+    <col min="5" max="5" width="11.69140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.3828125" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.53515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.53515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="16384" width="9.15234375" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -634,7 +637,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" ht="15.9" x14ac:dyDescent="0.45">
       <c r="A2" s="2" t="s">
         <v>8</v>
       </c>
@@ -660,7 +663,7 @@
         <v>647094308</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" ht="15.9" x14ac:dyDescent="0.45">
       <c r="A3" s="2" t="s">
         <v>8</v>
       </c>
@@ -686,7 +689,7 @@
         <v>908829627</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" ht="15.9" x14ac:dyDescent="0.45">
       <c r="A4" s="2" t="s">
         <v>8</v>
       </c>
@@ -712,7 +715,7 @@
         <v>875927684</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" ht="15.9" x14ac:dyDescent="0.45">
       <c r="A5" s="2" t="s">
         <v>8</v>
       </c>
@@ -738,7 +741,7 @@
         <v>225710755</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" ht="15.9" x14ac:dyDescent="0.45">
       <c r="A6" s="2" t="s">
         <v>8</v>
       </c>
@@ -764,7 +767,7 @@
         <v>972054725</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" ht="15.9" x14ac:dyDescent="0.45">
       <c r="A7" s="2" t="s">
         <v>8</v>
       </c>
@@ -790,7 +793,7 @@
         <v>722655386</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" ht="15.9" x14ac:dyDescent="0.45">
       <c r="A8" s="2" t="s">
         <v>8</v>
       </c>
@@ -816,7 +819,7 @@
         <v>727363340</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" ht="15.9" x14ac:dyDescent="0.45">
       <c r="A9" s="2" t="s">
         <v>8</v>
       </c>
@@ -842,7 +845,7 @@
         <v>426419003</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" ht="15.9" x14ac:dyDescent="0.45">
       <c r="A10" s="2" t="s">
         <v>8</v>
       </c>
@@ -868,7 +871,7 @@
         <v>403725253</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" ht="15.9" x14ac:dyDescent="0.45">
       <c r="A11" s="2" t="s">
         <v>8</v>
       </c>
@@ -894,7 +897,7 @@
         <v>647094308</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" ht="15.9" x14ac:dyDescent="0.45">
       <c r="A12" s="2" t="s">
         <v>8</v>
       </c>
@@ -920,7 +923,7 @@
         <v>908829627</v>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" ht="15.9" x14ac:dyDescent="0.45">
       <c r="A13" s="2" t="s">
         <v>8</v>
       </c>
@@ -946,7 +949,7 @@
         <v>875927684</v>
       </c>
     </row>
-    <row r="14" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" ht="15.9" x14ac:dyDescent="0.45">
       <c r="A14" s="2" t="s">
         <v>8</v>
       </c>
@@ -972,7 +975,7 @@
         <v>225710755</v>
       </c>
     </row>
-    <row r="15" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" ht="15.9" x14ac:dyDescent="0.45">
       <c r="A15" s="2" t="s">
         <v>8</v>
       </c>
@@ -998,7 +1001,7 @@
         <v>972054725</v>
       </c>
     </row>
-    <row r="16" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" ht="15.9" x14ac:dyDescent="0.45">
       <c r="A16" s="2" t="s">
         <v>8</v>
       </c>
@@ -1024,7 +1027,7 @@
         <v>722655386</v>
       </c>
     </row>
-    <row r="17" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" ht="15.9" x14ac:dyDescent="0.45">
       <c r="A17" s="2" t="s">
         <v>8</v>
       </c>
@@ -1050,7 +1053,7 @@
         <v>727363340</v>
       </c>
     </row>
-    <row r="18" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" ht="15.9" x14ac:dyDescent="0.45">
       <c r="A18" s="2" t="s">
         <v>8</v>
       </c>
@@ -1076,7 +1079,7 @@
         <v>426419003</v>
       </c>
     </row>
-    <row r="19" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" ht="15.9" x14ac:dyDescent="0.45">
       <c r="A19" s="2" t="s">
         <v>8</v>
       </c>
@@ -1102,7 +1105,7 @@
         <v>403725253</v>
       </c>
     </row>
-    <row r="20" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" ht="15.9" x14ac:dyDescent="0.45">
       <c r="A20" s="2" t="s">
         <v>8</v>
       </c>
@@ -1128,7 +1131,7 @@
         <v>647094308</v>
       </c>
     </row>
-    <row r="21" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" ht="15.9" x14ac:dyDescent="0.45">
       <c r="A21" s="2" t="s">
         <v>8</v>
       </c>
@@ -1154,7 +1157,7 @@
         <v>908829627</v>
       </c>
     </row>
-    <row r="22" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" ht="15.9" x14ac:dyDescent="0.45">
       <c r="A22" s="2" t="s">
         <v>8</v>
       </c>
@@ -1180,7 +1183,7 @@
         <v>875927684</v>
       </c>
     </row>
-    <row r="23" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" ht="15.9" x14ac:dyDescent="0.45">
       <c r="A23" s="2" t="s">
         <v>8</v>
       </c>
@@ -1206,7 +1209,7 @@
         <v>225710755</v>
       </c>
     </row>
-    <row r="24" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" ht="15.9" x14ac:dyDescent="0.45">
       <c r="A24" s="2" t="s">
         <v>8</v>
       </c>
@@ -1232,7 +1235,7 @@
         <v>972054725</v>
       </c>
     </row>
-    <row r="25" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8" ht="15.9" x14ac:dyDescent="0.45">
       <c r="A25" s="2" t="s">
         <v>8</v>
       </c>
@@ -1258,7 +1261,7 @@
         <v>722655386</v>
       </c>
     </row>
-    <row r="26" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8" ht="15.9" x14ac:dyDescent="0.45">
       <c r="A26" s="2" t="s">
         <v>8</v>
       </c>
@@ -1284,7 +1287,7 @@
         <v>727363340</v>
       </c>
     </row>
-    <row r="27" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8" ht="15.9" x14ac:dyDescent="0.45">
       <c r="A27" s="2" t="s">
         <v>8</v>
       </c>
@@ -1310,7 +1313,7 @@
         <v>426419003</v>
       </c>
     </row>
-    <row r="28" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8" ht="15.9" x14ac:dyDescent="0.45">
       <c r="A28" s="2" t="s">
         <v>8</v>
       </c>
@@ -1337,9 +1340,13 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="H1:H28" xr:uid="{5EBB363B-B62F-42A3-A89D-99F2C4FC4A0B}"/>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <headerFooter>
+    <oddFooter xml:space="preserve">&amp;C_x000D_&amp;1#&amp;"Calibri"&amp;10&amp;K000000 Public </oddFooter>
+  </headerFooter>
 </worksheet>
 </file>
 
@@ -1351,22 +1358,22 @@
       <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.15234375" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="1" max="1" width="10" style="2" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11" style="2" customWidth="1"/>
-    <col min="3" max="3" width="13.42578125" style="2" customWidth="1"/>
-    <col min="4" max="4" width="16.140625" style="2" customWidth="1"/>
-    <col min="5" max="5" width="16.5703125" style="2" customWidth="1"/>
-    <col min="6" max="6" width="15.28515625" style="2" customWidth="1"/>
-    <col min="7" max="7" width="16.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.3828125" style="2" customWidth="1"/>
+    <col min="4" max="4" width="16.15234375" style="2" customWidth="1"/>
+    <col min="5" max="5" width="16.53515625" style="2" customWidth="1"/>
+    <col min="6" max="6" width="15.3046875" style="2" customWidth="1"/>
+    <col min="7" max="7" width="16.84375" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.53515625" style="2" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="13" style="2" customWidth="1"/>
-    <col min="10" max="10" width="14.42578125" style="2" customWidth="1"/>
-    <col min="11" max="16384" width="9.140625" style="2"/>
+    <col min="10" max="10" width="14.3828125" style="2" customWidth="1"/>
+    <col min="11" max="16384" width="9.15234375" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1398,7 +1405,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" ht="15.9" x14ac:dyDescent="0.45">
       <c r="A2" s="2" t="s">
         <v>8</v>
       </c>
@@ -1430,7 +1437,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" ht="15.9" x14ac:dyDescent="0.45">
       <c r="A3" s="2" t="s">
         <v>8</v>
       </c>
@@ -1462,7 +1469,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" ht="15.9" x14ac:dyDescent="0.45">
       <c r="A4" s="2" t="s">
         <v>8</v>
       </c>
@@ -1494,7 +1501,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" ht="15.9" x14ac:dyDescent="0.45">
       <c r="A5" s="2" t="s">
         <v>8</v>
       </c>
@@ -1526,7 +1533,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" ht="15.9" x14ac:dyDescent="0.45">
       <c r="A6" s="2" t="s">
         <v>8</v>
       </c>
@@ -1558,7 +1565,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" ht="15.9" x14ac:dyDescent="0.45">
       <c r="A7" s="2" t="s">
         <v>8</v>
       </c>
@@ -1590,7 +1597,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" ht="15.9" x14ac:dyDescent="0.45">
       <c r="A8" s="2" t="s">
         <v>8</v>
       </c>
@@ -1622,7 +1629,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" ht="15.9" x14ac:dyDescent="0.45">
       <c r="A9" s="2" t="s">
         <v>8</v>
       </c>
@@ -1654,7 +1661,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" ht="15.9" x14ac:dyDescent="0.45">
       <c r="A10" s="2" t="s">
         <v>8</v>
       </c>
@@ -1690,6 +1697,9 @@
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <headerFooter>
+    <oddFooter xml:space="preserve">&amp;C_x000D_&amp;1#&amp;"Calibri"&amp;10&amp;K000000 Public </oddFooter>
+  </headerFooter>
 </worksheet>
 </file>
 
@@ -1697,24 +1707,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DBBD98E4-C59C-4D69-AC43-41574FFBEA9B}">
   <dimension ref="A1:H28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="M16" sqref="M16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.15234375" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="1" max="1" width="10" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.3828125" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.3046875" style="2" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="15" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="9" max="16384" width="9.140625" style="2"/>
+    <col min="5" max="5" width="11.69140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.3828125" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.53515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.53515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="16384" width="9.15234375" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1740,7 +1750,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" ht="15.9" x14ac:dyDescent="0.45">
       <c r="A2" s="2" t="s">
         <v>8</v>
       </c>
@@ -1766,7 +1776,7 @@
         <v>647094308</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" ht="15.9" x14ac:dyDescent="0.45">
       <c r="A3" s="2" t="s">
         <v>8</v>
       </c>
@@ -1792,7 +1802,7 @@
         <v>908829627</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" ht="15.9" x14ac:dyDescent="0.45">
       <c r="A4" s="2" t="s">
         <v>8</v>
       </c>
@@ -1818,7 +1828,7 @@
         <v>875927684</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" ht="15.9" x14ac:dyDescent="0.45">
       <c r="A5" s="2" t="s">
         <v>8</v>
       </c>
@@ -1844,7 +1854,7 @@
         <v>225710755</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" ht="15.9" x14ac:dyDescent="0.45">
       <c r="A6" s="2" t="s">
         <v>8</v>
       </c>
@@ -1870,7 +1880,7 @@
         <v>972054725</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" ht="15.9" x14ac:dyDescent="0.45">
       <c r="A7" s="2" t="s">
         <v>8</v>
       </c>
@@ -1896,7 +1906,7 @@
         <v>722655386</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" ht="15.9" x14ac:dyDescent="0.45">
       <c r="A8" s="2" t="s">
         <v>8</v>
       </c>
@@ -1922,7 +1932,7 @@
         <v>727363340</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" ht="15.9" x14ac:dyDescent="0.45">
       <c r="A9" s="2" t="s">
         <v>8</v>
       </c>
@@ -1948,7 +1958,7 @@
         <v>426419003</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" ht="15.9" x14ac:dyDescent="0.45">
       <c r="A10" s="2" t="s">
         <v>8</v>
       </c>
@@ -1974,7 +1984,7 @@
         <v>403725253</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" ht="15.9" x14ac:dyDescent="0.45">
       <c r="A11" s="2" t="s">
         <v>8</v>
       </c>
@@ -2000,7 +2010,7 @@
         <v>647094308</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" ht="15.9" x14ac:dyDescent="0.45">
       <c r="A12" s="2" t="s">
         <v>8</v>
       </c>
@@ -2026,7 +2036,7 @@
         <v>908829627</v>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" ht="15.9" x14ac:dyDescent="0.45">
       <c r="A13" s="2" t="s">
         <v>8</v>
       </c>
@@ -2052,7 +2062,7 @@
         <v>875927684</v>
       </c>
     </row>
-    <row r="14" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" ht="15.9" x14ac:dyDescent="0.45">
       <c r="A14" s="2" t="s">
         <v>8</v>
       </c>
@@ -2078,7 +2088,7 @@
         <v>225710755</v>
       </c>
     </row>
-    <row r="15" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" ht="15.9" x14ac:dyDescent="0.45">
       <c r="A15" s="2" t="s">
         <v>8</v>
       </c>
@@ -2104,7 +2114,7 @@
         <v>972054725</v>
       </c>
     </row>
-    <row r="16" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" ht="15.9" x14ac:dyDescent="0.45">
       <c r="A16" s="2" t="s">
         <v>8</v>
       </c>
@@ -2130,7 +2140,7 @@
         <v>722655386</v>
       </c>
     </row>
-    <row r="17" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" ht="15.9" x14ac:dyDescent="0.45">
       <c r="A17" s="2" t="s">
         <v>8</v>
       </c>
@@ -2156,7 +2166,7 @@
         <v>727363340</v>
       </c>
     </row>
-    <row r="18" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" ht="15.9" x14ac:dyDescent="0.45">
       <c r="A18" s="2" t="s">
         <v>8</v>
       </c>
@@ -2182,7 +2192,7 @@
         <v>426419003</v>
       </c>
     </row>
-    <row r="19" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" ht="15.9" x14ac:dyDescent="0.45">
       <c r="A19" s="2" t="s">
         <v>8</v>
       </c>
@@ -2208,7 +2218,7 @@
         <v>403725253</v>
       </c>
     </row>
-    <row r="20" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" ht="15.9" x14ac:dyDescent="0.45">
       <c r="A20" s="2" t="s">
         <v>8</v>
       </c>
@@ -2234,7 +2244,7 @@
         <v>647094308</v>
       </c>
     </row>
-    <row r="21" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" ht="15.9" x14ac:dyDescent="0.45">
       <c r="A21" s="2" t="s">
         <v>8</v>
       </c>
@@ -2260,7 +2270,7 @@
         <v>908829627</v>
       </c>
     </row>
-    <row r="22" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" ht="15.9" x14ac:dyDescent="0.45">
       <c r="A22" s="2" t="s">
         <v>8</v>
       </c>
@@ -2286,7 +2296,7 @@
         <v>875927684</v>
       </c>
     </row>
-    <row r="23" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" ht="15.9" x14ac:dyDescent="0.45">
       <c r="A23" s="2" t="s">
         <v>8</v>
       </c>
@@ -2312,7 +2322,7 @@
         <v>225710755</v>
       </c>
     </row>
-    <row r="24" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" ht="15.9" x14ac:dyDescent="0.45">
       <c r="A24" s="2" t="s">
         <v>8</v>
       </c>
@@ -2338,7 +2348,7 @@
         <v>972054725</v>
       </c>
     </row>
-    <row r="25" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8" ht="15.9" x14ac:dyDescent="0.45">
       <c r="A25" s="2" t="s">
         <v>8</v>
       </c>
@@ -2364,7 +2374,7 @@
         <v>722655386</v>
       </c>
     </row>
-    <row r="26" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8" ht="15.9" x14ac:dyDescent="0.45">
       <c r="A26" s="2" t="s">
         <v>8</v>
       </c>
@@ -2390,7 +2400,7 @@
         <v>727363340</v>
       </c>
     </row>
-    <row r="27" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8" ht="15.9" x14ac:dyDescent="0.45">
       <c r="A27" s="2" t="s">
         <v>8</v>
       </c>
@@ -2416,7 +2426,7 @@
         <v>426419003</v>
       </c>
     </row>
-    <row r="28" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8" ht="15.9" x14ac:dyDescent="0.45">
       <c r="A28" s="2" t="s">
         <v>8</v>
       </c>
@@ -2445,5 +2455,8 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <headerFooter>
+    <oddFooter xml:space="preserve">&amp;C_x000D_&amp;1#&amp;"Calibri"&amp;10&amp;K000000 Public </oddFooter>
+  </headerFooter>
 </worksheet>
 </file>
</xml_diff>